<commit_message>
[A] add fitting pkl file
</commit_message>
<xml_diff>
--- a/out/ml_model_result/index.xlsx
+++ b/out/ml_model_result/index.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toranosuke/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toranosuke/Desktop/DoV_ML/out/ml_model_result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4686435-1325-954A-A869-A98FD34A7BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{631B7170-0AD2-034D-B874-1B0D8C0D679C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{C39C54D5-2076-D54E-9F47-FB65B7F2F040}"/>
+    <workbookView xWindow="-36160" yWindow="740" windowWidth="34640" windowHeight="21100" xr2:uid="{C39C54D5-2076-D54E-9F47-FB65B7F2F040}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$50</definedName>
+    <definedName name="Z_0848F74C_49F2_314A_990A_863A30F08478_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$L$50</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <customWorkbookViews>
+    <customWorkbookView name="加藤虎之介 - 個人用ビュー" guid="{0848F74C-49F2-314A-990A-863A30F08478}" mergeInterval="0" personalView="1" xWindow="-1808" yWindow="37" windowWidth="1732" windowHeight="1055" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,15 +412,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -428,6 +423,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,6 +448,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A0BFAD44-70EE-3A42-B8A6-AE42FE54191B}" diskRevisions="1" revisionId="1" version="2">
+  <header guid="{6F8A9ED9-8E8D-A14F-9087-A12CDCF34D19}" dateTime="2021-11-29T01:29:10" maxSheetId="2" userName="加藤虎之介" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A0BFAD44-70EE-3A42-B8A6-AE42FE54191B}" dateTime="2021-11-29T01:32:43" maxSheetId="2" userName="加藤虎之介" r:id="rId2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{0848F74C-49F2-314A-990A-863A30F08478}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_0848F74C_49F2_314A_990A_863A30F08478_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$L$50</formula>
+    <oldFormula>Sheet1!$A$1:$L$50</oldFormula>
+  </rdn>
+  <rcv guid="{0848F74C-49F2-314A-990A-863A30F08478}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -747,7 +785,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -755,7 +793,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="15" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="20.140625" customWidth="1"/>
@@ -766,44 +804,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1" t="s">
         <v>60</v>
       </c>
@@ -830,7 +868,7 @@
       <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="7" t="b">
+      <c r="D3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E3">
@@ -865,7 +903,7 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="7" t="b">
+      <c r="D4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E4">
@@ -900,7 +938,7 @@
       <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="7" t="b">
+      <c r="D5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E5">
@@ -935,7 +973,7 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="7" t="b">
+      <c r="D6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E6">
@@ -970,7 +1008,7 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="7" t="b">
+      <c r="D7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E7">
@@ -1005,7 +1043,7 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="7" t="b">
+      <c r="D8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E8">
@@ -1034,78 +1072,78 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="9">
-        <v>0</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="6">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="D9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="6">
         <v>0.87968749999999996</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>7.3677413798343598E-3</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="6">
         <v>0.54732142857142796</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="6">
         <v>3.67252471730194E-2</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="6">
         <v>0.16126860402187701</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="6">
         <v>0.112261328011881</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="9">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
+      <c r="A10" s="6">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="D10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="6">
         <v>0.876388888888888</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="6">
         <v>1.7010345435994299E-3</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="6">
         <v>0.50734126984126904</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="6">
         <v>8.9417891581299608E-3</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="6">
         <v>2.9011439738680901E-2</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="6">
         <v>3.5582567372087703E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="9" customFormat="1">
+    <row r="11" spans="1:12" s="6" customFormat="1">
       <c r="A11"/>
       <c r="B11">
         <v>1</v>
@@ -1113,7 +1151,7 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="b">
+      <c r="D11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1141,7 +1179,7 @@
         <v>8.4962047621615994E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="9" customFormat="1">
+    <row r="12" spans="1:12" s="6" customFormat="1">
       <c r="A12"/>
       <c r="B12">
         <v>1</v>
@@ -1149,7 +1187,7 @@
       <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="7" t="b">
+      <c r="D12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1184,7 +1222,7 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="7" t="b">
+      <c r="D13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1219,7 +1257,7 @@
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="7" t="b">
+      <c r="D14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
@@ -1254,7 +1292,7 @@
       <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="7" t="b">
+      <c r="D15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E15" t="s">
@@ -1289,7 +1327,7 @@
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="7" t="b">
+      <c r="D16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
@@ -1324,7 +1362,7 @@
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="7" t="b">
+      <c r="D17" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
@@ -1359,7 +1397,7 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="7" t="b">
+      <c r="D18" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="s">
@@ -1394,7 +1432,7 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="7" t="b">
+      <c r="D19" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
@@ -1429,7 +1467,7 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7" t="b">
+      <c r="D20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="s">
@@ -1464,7 +1502,7 @@
       <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="7" t="b">
+      <c r="D21" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1499,7 +1537,7 @@
       <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="7" t="b">
+      <c r="D22" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
@@ -1534,7 +1572,7 @@
       <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="7" t="b">
+      <c r="D23" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1569,7 +1607,7 @@
       <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="7" t="b">
+      <c r="D24" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="s">
@@ -1604,7 +1642,7 @@
       <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="7" t="b">
+      <c r="D25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="s">
@@ -1639,7 +1677,7 @@
       <c r="C26" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="7" t="b">
+      <c r="D26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="s">
@@ -1674,7 +1712,7 @@
       <c r="C27" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="7" t="b">
+      <c r="D27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1709,7 +1747,7 @@
       <c r="C28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="7" t="b">
+      <c r="D28" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1744,7 +1782,7 @@
       <c r="C29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="7" t="b">
+      <c r="D29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="s">
@@ -1779,7 +1817,7 @@
       <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="7" t="b">
+      <c r="D30" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E30" t="s">
@@ -1814,7 +1852,7 @@
       <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="7" t="b">
+      <c r="D31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="s">
@@ -1849,7 +1887,7 @@
       <c r="C32" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="7" t="b">
+      <c r="D32" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="s">
@@ -1884,7 +1922,7 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="7" t="b">
+      <c r="D33" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E33" t="s">
@@ -1919,7 +1957,7 @@
       <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="7" t="b">
+      <c r="D34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="s">
@@ -1954,7 +1992,7 @@
       <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="7" t="b">
+      <c r="D35" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1989,7 +2027,7 @@
       <c r="C36" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="7" t="b">
+      <c r="D36" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E36" t="s">
@@ -2027,7 +2065,7 @@
       <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="7" t="b">
+      <c r="D37" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E37" t="s">
@@ -2062,7 +2100,7 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="7" t="b">
+      <c r="D38" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="s">
@@ -2097,7 +2135,7 @@
       <c r="C39" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="7" t="b">
+      <c r="D39" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E39" t="s">
@@ -2135,7 +2173,7 @@
       <c r="C40" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="7" t="b">
+      <c r="D40" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E40" t="s">
@@ -2170,7 +2208,7 @@
       <c r="C41" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="7" t="b">
+      <c r="D41" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2208,7 +2246,7 @@
       <c r="C42" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="7" t="b">
+      <c r="D42" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E42" t="s">
@@ -2246,7 +2284,7 @@
       <c r="C43" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="7" t="b">
+      <c r="D43" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E43" t="s">
@@ -2284,7 +2322,7 @@
       <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="7" t="b">
+      <c r="D44" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E44" t="s">
@@ -2322,7 +2360,7 @@
       <c r="C45" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="7" t="b">
+      <c r="D45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E45" t="s">
@@ -2360,7 +2398,7 @@
       <c r="C46" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="7" t="b">
+      <c r="D46" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E46" t="s">
@@ -2398,7 +2436,7 @@
       <c r="C47" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="7" t="b">
+      <c r="D47" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E47" t="s">
@@ -2436,7 +2474,7 @@
       <c r="C48" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="7" t="b">
+      <c r="D48" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E48" t="s">
@@ -2474,7 +2512,7 @@
       <c r="C49" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="7" t="b">
+      <c r="D49" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E49" t="s">
@@ -2512,7 +2550,7 @@
       <c r="C50" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="8"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="2"/>
     </row>
     <row r="1048576" spans="5:5">
@@ -2529,6 +2567,18 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C50">
     <sortCondition ref="C1:C50"/>
   </sortState>
+  <customSheetViews>
+    <customSheetView guid="{0848F74C-49F2-314A-990A-863A30F08478}" scale="94" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:L50" xr:uid="{B9EF4E10-2359-3546-89E9-D98D539152BA}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L50">
+          <sortCondition descending="1" ref="G1:G50"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="9">
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>